<commit_message>
Reunion informal 2013-09-23 .pptx
</commit_message>
<xml_diff>
--- a/docs/2013-09-21 Movies Data.xlsx
+++ b/docs/2013-09-21 Movies Data.xlsx
@@ -199,7 +199,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +214,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -223,12 +231,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -239,9 +262,13 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -540,7 +567,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -552,288 +579,288 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>112</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>119</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>96</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>95</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>118</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>109</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>109</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>85</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>131</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>90</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="2" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>